<commit_message>
Working screenshot and link count
</commit_message>
<xml_diff>
--- a/data/sheet.xlsx
+++ b/data/sheet.xlsx
@@ -198,7 +198,7 @@
     </r>
   </si>
   <si>
-    <t>Test</t>
+    <t>imageUrl</t>
   </si>
   <si>
     <t>WC-789036</t>
@@ -1375,7 +1375,7 @@
         <v>15</v>
       </c>
       <c r="U2" s="17">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="V2" s="18" t="s">
         <v>42</v>
@@ -1471,7 +1471,7 @@
         <v>15</v>
       </c>
       <c r="U3" s="17">
-        <v>0</v>
+        <v>118</v>
       </c>
       <c r="V3" s="18" t="s">
         <v>42</v>
@@ -1565,7 +1565,7 @@
         <v>3</v>
       </c>
       <c r="U4" s="17">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="V4" s="18" t="s">
         <v>42</v>
@@ -1661,7 +1661,7 @@
         <v>3</v>
       </c>
       <c r="U5" s="17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V5" s="18" t="s">
         <v>42</v>
@@ -1757,7 +1757,7 @@
         <v>5</v>
       </c>
       <c r="U6" s="17">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="V6" s="18" t="s">
         <v>42</v>
@@ -1953,7 +1953,7 @@
         <v>3</v>
       </c>
       <c r="U8" s="17">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="V8" s="18" t="s">
         <v>42</v>

</xml_diff>